<commit_message>
automation test NUnit for Sigin and Register
</commit_message>
<xml_diff>
--- a/server/server.Tests/Report/WhiteBox_Signin_Report.xlsx
+++ b/server/server.Tests/Report/WhiteBox_Signin_Report.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="WhiteBox_Signin_Results" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Signin_Test_Summary" sheetId="1" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -19,70 +19,67 @@
     <x:t>Test Case</x:t>
   </x:si>
   <x:si>
-    <x:t>Step Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Expected Result</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Actual Result</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Status</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TC01: Account Not Found</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kiểm tra sự tồn tại của Email</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Throw ErrorHandlingException</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Exception Thrown</x:t>
+    <x:t>Exp StatusCode</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Act StatusCode</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Expected Message/Data</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Actual Message/Data</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Final Status</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TC01: Missing Email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DTO Error</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email không được để trống!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email Is Required!</x:t>
   </x:si>
   <x:si>
     <x:t>FAIL</x:t>
   </x:si>
   <x:si>
-    <x:t>So khớp thông báo lỗi</x:t>
+    <x:t>TC02: Wrong Email Format</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vui lòng nhập đúng định dạng!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PASS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TC03: Account Not Found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>400</x:t>
   </x:si>
   <x:si>
     <x:t>Tài khoản không tồn tại!</x:t>
   </x:si>
   <x:si>
-    <x:t>PASS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TC02: Invalid Password</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kiểm tra mật khẩu</x:t>
+    <x:t>TC04: Invalid Password</x:t>
   </x:si>
   <x:si>
     <x:t>Sai mật khẩu!</x:t>
   </x:si>
   <x:si>
-    <x:t>TC03: Signin Success</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kiểm tra dữ liệu UserName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Văn A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kiểm tra thiết lập Cookie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>True</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Xác minh lưu RefreshToken</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Called Once</x:t>
+    <x:t>TC05: Signin Success</x:t>
+  </x:si>
+  <x:si>
+    <x:t>200</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User: abc, Role: Doctor</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -481,20 +478,20 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E8"/>
+  <x:dimension ref="A1:F6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="23.853482" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="26.282054" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="28.424911" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="22.996339" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="6.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="24.853482" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="14.853482" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="14.567768" style="0" customWidth="1"/>
+    <x:col min="4" max="5" width="28.710625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="11.139196" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -510,13 +507,16 @@
       <x:c r="E1" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>7</x:v>
@@ -524,110 +524,91 @@
       <x:c r="D2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E2" s="2" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:5">
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E3" s="3" t="s">
         <x:v>12</x:v>
       </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F3" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
     </x:row>
-    <x:row r="4" spans="1:5">
+    <x:row r="4" spans="1:6">
       <x:c r="A4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F4" s="3" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E4" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
     </x:row>
-    <x:row r="5" spans="1:5">
+    <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E5" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F5" s="3" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:5">
+    <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E6" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E7" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E8" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="E6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F6" s="3" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>